<commit_message>
Removed deprecated FusedLocationAPI and using FusedLocationProviderClient instead
</commit_message>
<xml_diff>
--- a/DTT-Test-Hour-Log.xlsx
+++ b/DTT-Test-Hour-Log.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10319"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meng/Projects/Pechhulp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A74D1E5D-E3B3-584F-B134-0FE33D1DF0B3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21E530A0-B068-614C-A71C-E175CE91F80C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12840" yWindow="0" windowWidth="12760" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12860" yWindow="460" windowWidth="12740" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DTT Test Hour Log" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>Subject</t>
   </si>
@@ -145,24 +145,9 @@
     <t>Scaling images</t>
   </si>
   <si>
-    <t>Status bar  wrong colour</t>
-  </si>
-  <si>
-    <t>Toolbar title</t>
-  </si>
-  <si>
-    <t>Back button is incorrect</t>
-  </si>
-  <si>
-    <t>Info text link wrong colour</t>
-  </si>
-  <si>
     <t xml:space="preserve">Call popup </t>
   </si>
   <si>
-    <t>Styles and colours</t>
-  </si>
-  <si>
     <t>Tablet layout</t>
   </si>
   <si>
@@ -173,6 +158,24 @@
   </si>
   <si>
     <t>FusedLocationAPI is deprecated</t>
+  </si>
+  <si>
+    <t>Tried several things (scaling a bitmap, using a framelayout instead of a linearlayout) but eventually went with with centerCrop for the main image in an image view (found out you can't scale a background image - unless it's a bitmap. For the info image just made sure adjustViewBounds was set to true. Image view was in front of action bar</t>
+  </si>
+  <si>
+    <t>Simple after figuring out how to use the native toolbar.</t>
+  </si>
+  <si>
+    <t>Toolbar title. Back button is incorrect.</t>
+  </si>
+  <si>
+    <t>Had problems with transparency and gravity. Removed the calling button when popup came up and appeared again when closed.</t>
+  </si>
+  <si>
+    <t>Status bar  wrong colour. Info text link wrong colour. Styles and colours.</t>
+  </si>
+  <si>
+    <t>Took a long time to figure out how themes worked. Changed accented colours. Removed white as hardcoded and put it in colors.</t>
   </si>
 </sst>
 </file>
@@ -1776,10 +1779,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A11" zoomScale="156" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="6.5" defaultRowHeight="15" customHeight="1"/>
@@ -2018,7 +2021,7 @@
       <c r="E15" s="3"/>
       <c r="F15" s="5"/>
     </row>
-    <row r="16" spans="1:6" ht="34">
+    <row r="16" spans="1:6" ht="23">
       <c r="A16" s="19" t="s">
         <v>15</v>
       </c>
@@ -2034,69 +2037,93 @@
       <c r="E16" s="3"/>
       <c r="F16" s="5"/>
     </row>
-    <row r="17" spans="1:6" ht="16">
+    <row r="17" spans="1:6" ht="45">
       <c r="A17" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="17"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="20"/>
+      <c r="B17" s="17">
+        <v>1</v>
+      </c>
+      <c r="C17" s="18">
+        <v>43179</v>
+      </c>
+      <c r="D17" s="20" t="s">
+        <v>38</v>
+      </c>
       <c r="E17" s="3"/>
       <c r="F17" s="5"/>
     </row>
-    <row r="18" spans="1:6" ht="16">
+    <row r="18" spans="1:6" ht="24" customHeight="1">
       <c r="A18" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="B18" s="17"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="20"/>
+        <v>40</v>
+      </c>
+      <c r="B18" s="17">
+        <v>1.5</v>
+      </c>
+      <c r="C18" s="18">
+        <v>43197</v>
+      </c>
+      <c r="D18" s="20" t="s">
+        <v>39</v>
+      </c>
       <c r="E18" s="3"/>
       <c r="F18" s="5"/>
     </row>
-    <row r="19" spans="1:6" ht="16">
+    <row r="19" spans="1:6" ht="23">
       <c r="A19" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="B19" s="17"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="20"/>
+        <v>42</v>
+      </c>
+      <c r="B19" s="17">
+        <v>2</v>
+      </c>
+      <c r="C19" s="18">
+        <v>43197</v>
+      </c>
+      <c r="D19" s="20" t="s">
+        <v>43</v>
+      </c>
       <c r="E19" s="3"/>
       <c r="F19" s="5"/>
     </row>
-    <row r="20" spans="1:6" ht="16">
+    <row r="20" spans="1:6" ht="23">
       <c r="A20" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="B20" s="17"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="20"/>
+        <v>33</v>
+      </c>
+      <c r="B20" s="17">
+        <v>2</v>
+      </c>
+      <c r="C20" s="18">
+        <v>43199</v>
+      </c>
+      <c r="D20" s="20" t="s">
+        <v>41</v>
+      </c>
       <c r="E20" s="3"/>
       <c r="F20" s="5"/>
     </row>
-    <row r="21" spans="1:6" ht="16">
+    <row r="21" spans="1:6" ht="17" customHeight="1">
       <c r="A21" s="19" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B21" s="17"/>
       <c r="C21" s="18"/>
-      <c r="D21" s="20"/>
+      <c r="D21" s="15"/>
       <c r="E21" s="3"/>
       <c r="F21" s="5"/>
     </row>
-    <row r="22" spans="1:6" ht="16">
+    <row r="22" spans="1:6" ht="17" customHeight="1">
       <c r="A22" s="19" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B22" s="17"/>
       <c r="C22" s="18"/>
-      <c r="D22" s="20"/>
+      <c r="D22" s="15"/>
       <c r="E22" s="3"/>
       <c r="F22" s="5"/>
     </row>
     <row r="23" spans="1:6" ht="17" customHeight="1">
       <c r="A23" s="19" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B23" s="17"/>
       <c r="C23" s="18"/>
@@ -2106,7 +2133,7 @@
     </row>
     <row r="24" spans="1:6" ht="17" customHeight="1">
       <c r="A24" s="19" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B24" s="17"/>
       <c r="C24" s="18"/>
@@ -2115,87 +2142,57 @@
       <c r="F24" s="5"/>
     </row>
     <row r="25" spans="1:6" ht="17" customHeight="1">
-      <c r="A25" s="19" t="s">
-        <v>40</v>
-      </c>
+      <c r="A25" s="19"/>
       <c r="B25" s="17"/>
       <c r="C25" s="18"/>
       <c r="D25" s="15"/>
       <c r="E25" s="3"/>
       <c r="F25" s="5"/>
     </row>
-    <row r="26" spans="1:6" ht="17" customHeight="1">
-      <c r="A26" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="B26" s="17"/>
-      <c r="C26" s="18"/>
-      <c r="D26" s="15"/>
-      <c r="E26" s="3"/>
+    <row r="26" spans="1:6" ht="16" customHeight="1">
+      <c r="A26" s="11"/>
+      <c r="B26" s="12"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="4"/>
       <c r="F26" s="5"/>
     </row>
-    <row r="27" spans="1:6" ht="17" customHeight="1">
-      <c r="A27" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="B27" s="17"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="15"/>
-      <c r="E27" s="3"/>
+    <row r="27" spans="1:6" ht="16" customHeight="1">
+      <c r="A27" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27" s="14">
+        <f>SUM(B4:B25)</f>
+        <v>48.5</v>
+      </c>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
       <c r="F27" s="5"/>
     </row>
-    <row r="28" spans="1:6" ht="17" customHeight="1">
-      <c r="A28" s="19"/>
-      <c r="B28" s="17"/>
-      <c r="C28" s="18"/>
-      <c r="D28" s="15"/>
-      <c r="E28" s="3"/>
+    <row r="28" spans="1:6" ht="16" customHeight="1">
+      <c r="A28" s="6"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
       <c r="F28" s="5"/>
     </row>
     <row r="29" spans="1:6" ht="16" customHeight="1">
-      <c r="A29" s="11"/>
-      <c r="B29" s="12"/>
-      <c r="C29" s="12"/>
-      <c r="D29" s="12"/>
+      <c r="A29" s="6"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
       <c r="E29" s="4"/>
       <c r="F29" s="5"/>
     </row>
     <row r="30" spans="1:6" ht="16" customHeight="1">
-      <c r="A30" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="B30" s="14">
-        <f>SUM(B4:B28)</f>
-        <v>42</v>
-      </c>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="5"/>
-    </row>
-    <row r="31" spans="1:6" ht="16" customHeight="1">
-      <c r="A31" s="6"/>
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="5"/>
-    </row>
-    <row r="32" spans="1:6" ht="16" customHeight="1">
-      <c r="A32" s="6"/>
-      <c r="B32" s="4"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="5"/>
-    </row>
-    <row r="33" spans="1:6" ht="16" customHeight="1">
-      <c r="A33" s="7"/>
-      <c r="B33" s="8"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="8"/>
-      <c r="F33" s="9"/>
+      <c r="A30" s="7"/>
+      <c r="B30" s="8"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="8"/>
+      <c r="F30" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Added shadows to buttons and toolbar; started with tablet view
</commit_message>
<xml_diff>
--- a/DTT-Test-Hour-Log.xlsx
+++ b/DTT-Test-Hour-Log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meng/Projects/Pechhulp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21E530A0-B068-614C-A71C-E175CE91F80C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3064B295-4AB5-C245-8621-69F0503DD654}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12860" yWindow="460" windowWidth="12740" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1920" yWindow="460" windowWidth="23680" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DTT Test Hour Log" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>Subject</t>
   </si>
@@ -151,15 +151,9 @@
     <t>Tablet layout</t>
   </si>
   <si>
-    <t>Odd animation when map opens</t>
-  </si>
-  <si>
     <t>Property names do not macth</t>
   </si>
   <si>
-    <t>FusedLocationAPI is deprecated</t>
-  </si>
-  <si>
     <t>Tried several things (scaling a bitmap, using a framelayout instead of a linearlayout) but eventually went with with centerCrop for the main image in an image view (found out you can't scale a background image - unless it's a bitmap. For the info image just made sure adjustViewBounds was set to true. Image view was in front of action bar</t>
   </si>
   <si>
@@ -176,6 +170,15 @@
   </si>
   <si>
     <t>Took a long time to figure out how themes worked. Changed accented colours. Removed white as hardcoded and put it in colors.</t>
+  </si>
+  <si>
+    <t>Odd animation when map opens, FusedLocationAPI is deprecated</t>
+  </si>
+  <si>
+    <t>Changed the map so it no longer used deprecated API (changed to FusedLocationProviderClient) and location listener.</t>
+  </si>
+  <si>
+    <t>Changed names using the conventions (m for member variables, object type start - e.g. btn for button - followed by object description - e.g. btnCall for call button.</t>
   </si>
 </sst>
 </file>
@@ -1781,8 +1784,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A11" zoomScale="156" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="156" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="6.5" defaultRowHeight="15" customHeight="1"/>
@@ -2048,14 +2051,14 @@
         <v>43179</v>
       </c>
       <c r="D17" s="20" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="5"/>
     </row>
     <row r="18" spans="1:6" ht="24" customHeight="1">
       <c r="A18" s="19" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B18" s="17">
         <v>1.5</v>
@@ -2064,14 +2067,14 @@
         <v>43197</v>
       </c>
       <c r="D18" s="20" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E18" s="3"/>
       <c r="F18" s="5"/>
     </row>
     <row r="19" spans="1:6" ht="23">
       <c r="A19" s="19" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B19" s="17">
         <v>2</v>
@@ -2080,7 +2083,7 @@
         <v>43197</v>
       </c>
       <c r="D19" s="20" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E19" s="3"/>
       <c r="F19" s="5"/>
@@ -2096,34 +2099,46 @@
         <v>43199</v>
       </c>
       <c r="D20" s="20" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E20" s="3"/>
       <c r="F20" s="5"/>
     </row>
-    <row r="21" spans="1:6" ht="17" customHeight="1">
+    <row r="21" spans="1:6" ht="23">
       <c r="A21" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="B21" s="17"/>
-      <c r="C21" s="18"/>
-      <c r="D21" s="15"/>
+        <v>42</v>
+      </c>
+      <c r="B21" s="17">
+        <v>2</v>
+      </c>
+      <c r="C21" s="18">
+        <v>43199</v>
+      </c>
+      <c r="D21" s="20" t="s">
+        <v>43</v>
+      </c>
       <c r="E21" s="3"/>
       <c r="F21" s="5"/>
     </row>
-    <row r="22" spans="1:6" ht="17" customHeight="1">
+    <row r="22" spans="1:6" ht="23">
       <c r="A22" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="B22" s="17"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="15"/>
+      <c r="B22" s="17">
+        <v>1</v>
+      </c>
+      <c r="C22" s="18">
+        <v>43199</v>
+      </c>
+      <c r="D22" s="20" t="s">
+        <v>44</v>
+      </c>
       <c r="E22" s="3"/>
       <c r="F22" s="5"/>
     </row>
     <row r="23" spans="1:6" ht="17" customHeight="1">
       <c r="A23" s="19" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B23" s="17"/>
       <c r="C23" s="18"/>
@@ -2132,9 +2147,7 @@
       <c r="F23" s="5"/>
     </row>
     <row r="24" spans="1:6" ht="17" customHeight="1">
-      <c r="A24" s="19" t="s">
-        <v>37</v>
-      </c>
+      <c r="A24" s="19"/>
       <c r="B24" s="17"/>
       <c r="C24" s="18"/>
       <c r="D24" s="15"/>
@@ -2163,7 +2176,7 @@
       </c>
       <c r="B27" s="14">
         <f>SUM(B4:B25)</f>
-        <v>48.5</v>
+        <v>51.5</v>
       </c>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>

</xml_diff>